<commit_message>
excel is creating content tests
</commit_message>
<xml_diff>
--- a/D:\test excel\book2.xlsx
+++ b/D:\test excel\book2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoeking/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C450E81F-825C-6D43-A6CC-F92E6FCF1537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B491156C-D934-484B-8980-19E29AF2E8CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="1000" windowWidth="25040" windowHeight="13560" xr2:uid="{2055FD3A-2EA6-1C4B-B8E8-796A70A86976}"/>
+    <workbookView xWindow="11300" yWindow="500" windowWidth="25040" windowHeight="13560" xr2:uid="{2055FD3A-2EA6-1C4B-B8E8-796A70A86976}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -171,8 +171,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,7 +524,7 @@
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -600,7 +601,7 @@
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>44408</v>
       </c>
       <c r="B2" t="s">

</xml_diff>

<commit_message>
aggregate values working in test
</commit_message>
<xml_diff>
--- a/D:\test excel\book2.xlsx
+++ b/D:\test excel\book2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoeking/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD33731-81C5-174C-8EA3-52629BB521E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E498F09-5F93-0148-AABB-90E078243E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11300" yWindow="500" windowWidth="25040" windowHeight="13560" xr2:uid="{2055FD3A-2EA6-1C4B-B8E8-796A70A86976}"/>
+    <workbookView xWindow="3020" yWindow="500" windowWidth="25040" windowHeight="13560" xr2:uid="{2055FD3A-2EA6-1C4B-B8E8-796A70A86976}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>DATE</t>
   </si>
@@ -124,12 +124,6 @@
   </si>
   <si>
     <t>Express lanes</t>
-  </si>
-  <si>
-    <t>Variant A</t>
-  </si>
-  <si>
-    <t>Winner (Express)</t>
   </si>
   <si>
     <t>With express lanes</t>
@@ -181,40 +175,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE6B8AF"/>
-          <bgColor rgb="FFE6B8AF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE6B8AF"/>
-          <bgColor rgb="FFE6B8AF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -526,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE35CBB7-C243-5F48-A300-DFB07CB17338}">
   <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -632,13 +593,13 @@
         <v>29</v>
       </c>
       <c r="J2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M2">
         <v>15819</v>
@@ -650,7 +611,7 @@
         <v>1.8499999999999999E-2</v>
       </c>
       <c r="P2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Q2">
         <v>15936</v>
@@ -682,7 +643,7 @@
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D3">
         <v>31755</v>
@@ -703,13 +664,13 @@
         <v>29</v>
       </c>
       <c r="J3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M3">
         <v>15819</v>
@@ -721,7 +682,7 @@
         <v>1.8499999999999999E-2</v>
       </c>
       <c r="P3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Q3">
         <v>15936</v>

</xml_diff>

<commit_message>
test model updated with tied counts
</commit_message>
<xml_diff>
--- a/D:\test excel\book2.xlsx
+++ b/D:\test excel\book2.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoeking/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E498F09-5F93-0148-AABB-90E078243E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24C916F-4218-F44C-91D7-EF3BE4CD4002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3020" yWindow="500" windowWidth="25040" windowHeight="13560" xr2:uid="{2055FD3A-2EA6-1C4B-B8E8-796A70A86976}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="65">
   <si>
     <t>DATE</t>
   </si>
@@ -50,10 +50,6 @@
     <t xml:space="preserve">TOTAL NUMBER OF RECIPIENTS </t>
   </si>
   <si>
-    <t>(ACOUSTIC NAME) 
-SENDER NAME</t>
-  </si>
-  <si>
     <t>JTK</t>
   </si>
   <si>
@@ -81,9 +77,6 @@
     <t>VARIANT A OPEN RATE (OPN/RCV)</t>
   </si>
   <si>
-    <t>VARIANT A CLICK RATE</t>
-  </si>
-  <si>
     <t>VARIANT B TEST</t>
   </si>
   <si>
@@ -93,9 +86,6 @@
     <t>VARIANT B OPEN RATE (OPN/RCV)</t>
   </si>
   <si>
-    <t>VARIANT B CLICK RATE</t>
-  </si>
-  <si>
     <t>VARIANT A OPENS</t>
   </si>
   <si>
@@ -133,6 +123,127 @@
   </si>
   <si>
     <t>Prospects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+EMAIL NAME</t>
+  </si>
+  <si>
+    <t>VARIANT A CLICK RATE (CLK/RCV)</t>
+  </si>
+  <si>
+    <t>VARIANT B CLICK RATE (CLK/RCV)</t>
+  </si>
+  <si>
+    <t>VARIANT A</t>
+  </si>
+  <si>
+    <t>TIED</t>
+  </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>Full List</t>
+  </si>
+  <si>
+    <t>All Graphic Stacey Abrams Through The Roof - DGA</t>
+  </si>
+  <si>
+    <t>jtk8087</t>
+  </si>
+  <si>
+    <t>Michelle Obama Through the Roof - FR - DGA</t>
+  </si>
+  <si>
+    <t>jtk7949b</t>
+  </si>
+  <si>
+    <t>VARIANT B</t>
+  </si>
+  <si>
+    <t>DSCC Style quote template with Newsom Recall w/ surrogate quotes - PET</t>
+  </si>
+  <si>
+    <t>jtk8112</t>
+  </si>
+  <si>
+    <t>Petition</t>
+  </si>
+  <si>
+    <t>"Add your name"
+vs.
+"Yes/No"</t>
+  </si>
+  <si>
+    <t>Add Your Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes/No </t>
+  </si>
+  <si>
+    <t>OG- Beto's call to protect vr- PET - DGA - jtk8066</t>
+  </si>
+  <si>
+    <t>jtk8066</t>
+  </si>
+  <si>
+    <t>"Sign the Petition" 
+vs. 
+"Yes/No"</t>
+  </si>
+  <si>
+    <t>Sign Petition</t>
+  </si>
+  <si>
+    <t>RF - ALL GRAPHIC Biden Approval - SU - DGA</t>
+  </si>
+  <si>
+    <t>jtk8123</t>
+  </si>
+  <si>
+    <t>Survey</t>
+  </si>
+  <si>
+    <t>"Yes/No"
+vs 
+"Approval/Neutral/Disapprove"</t>
+  </si>
+  <si>
+    <t>Yes/No</t>
+  </si>
+  <si>
+    <t>Approve/
+Neutral/
+Disapprove</t>
+  </si>
+  <si>
+    <t>OG - ALL GRAPHIC - Joe Biden's Call John Lewis Act - PET - DGA - jtk8063</t>
+  </si>
+  <si>
+    <t>jtk8063</t>
+  </si>
+  <si>
+    <t>"Yes/No"
+vs 
+"Very Much/Somewhat/Unsure/Not at all"</t>
+  </si>
+  <si>
+    <t>Agree (4 Choices)</t>
+  </si>
+  <si>
+    <t>OG - Michelle and Stacey VRA - SU - DGA - jtk8125</t>
+  </si>
+  <si>
+    <t>jtk8125</t>
+  </si>
+  <si>
+    <t>"Yes/No"
+vs 
+"Worried/Somewhat/Not at all"</t>
+  </si>
+  <si>
+    <t>Worried (3 Choices)</t>
   </si>
 </sst>
 </file>
@@ -175,7 +286,70 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9D9D9"/>
+          <bgColor rgb="FFD9D9D9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE6B8AF"/>
+          <bgColor rgb="FFE6B8AF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB6D7A8"/>
+          <bgColor rgb="FFB6D7A8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB6D7A8"/>
+          <bgColor rgb="FFB6D7A8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB6D7A8"/>
+          <bgColor rgb="FFB6D7A8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -485,15 +659,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE35CBB7-C243-5F48-A300-DFB07CB17338}">
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="15" max="15" width="25.5" customWidth="1"/>
+    <col min="19" max="19" width="27.33203125" customWidth="1"/>
+    <col min="20" max="20" width="23.83203125" customWidth="1"/>
+    <col min="21" max="21" width="19.33203125" customWidth="1"/>
+    <col min="23" max="23" width="36" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -507,203 +688,913 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
+        <v>31</v>
+      </c>
+      <c r="T1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44408</v>
       </c>
       <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2">
+        <v>175444</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G2" t="s">
         <v>24</v>
       </c>
-      <c r="D2">
-        <v>31755</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>25</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" t="s">
         <v>26</v>
       </c>
-      <c r="G2" t="s">
+      <c r="M2">
+        <v>87734</v>
+      </c>
+      <c r="N2">
+        <v>0.182</v>
+      </c>
+      <c r="O2">
+        <v>2E-3</v>
+      </c>
+      <c r="P2" t="s">
         <v>27</v>
       </c>
-      <c r="H2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2">
-        <v>15819</v>
-      </c>
-      <c r="N2">
-        <v>0.17960000000000001</v>
-      </c>
-      <c r="O2">
-        <v>1.8499999999999999E-2</v>
-      </c>
-      <c r="P2" t="s">
-        <v>30</v>
-      </c>
       <c r="Q2">
-        <v>15936</v>
+        <v>87710</v>
       </c>
       <c r="R2">
-        <v>0.18099999999999999</v>
+        <v>0.183</v>
       </c>
       <c r="S2">
-        <v>1.61E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="T2">
-        <v>15819</v>
+        <v>15955</v>
       </c>
       <c r="U2">
-        <v>6.7999999999999996E-3</v>
+        <v>6.7000000000000002E-3</v>
       </c>
       <c r="V2">
-        <v>15936</v>
+        <v>16055</v>
       </c>
       <c r="W2">
-        <v>5.3E-3</v>
+        <v>5.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44408</v>
       </c>
       <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3">
+        <v>1093536</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3">
-        <v>31755</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
         <v>25</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" t="s">
         <v>26</v>
       </c>
-      <c r="G3" t="s">
+      <c r="M3">
+        <v>546859</v>
+      </c>
+      <c r="N3">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="O3">
+        <v>1E-3</v>
+      </c>
+      <c r="P3" t="s">
         <v>27</v>
       </c>
-      <c r="H3" t="s">
+      <c r="Q3">
+        <v>546677</v>
+      </c>
+      <c r="R3">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="S3">
+        <v>1E-3</v>
+      </c>
+      <c r="T3">
+        <v>91532</v>
+      </c>
+      <c r="U3">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="V3">
+        <v>90880</v>
+      </c>
+      <c r="W3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>44408</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4">
+        <v>203130</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4">
+        <v>549388</v>
+      </c>
+      <c r="N4">
+        <v>0.186</v>
+      </c>
+      <c r="O4">
+        <v>2E-3</v>
+      </c>
+      <c r="P4" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q4">
+        <v>555589</v>
+      </c>
+      <c r="R4">
+        <v>0.188</v>
+      </c>
+      <c r="S4">
+        <v>2E-3</v>
+      </c>
+      <c r="T4">
+        <v>101999</v>
+      </c>
+      <c r="U4">
+        <v>1.8E-3</v>
+      </c>
+      <c r="V4">
+        <v>103033</v>
+      </c>
+      <c r="W4">
+        <v>1.6999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>44408</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5">
+        <v>215446</v>
+      </c>
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5">
+        <v>646425</v>
+      </c>
+      <c r="N5">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="O5">
+        <v>1E-3</v>
+      </c>
+      <c r="P5" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q5">
+        <v>649239</v>
+      </c>
+      <c r="R5">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="S5">
+        <v>2E-3</v>
+      </c>
+      <c r="T5">
+        <v>109070</v>
+      </c>
+      <c r="U5">
+        <v>2.0999999999999999E-3</v>
+      </c>
+      <c r="V5">
+        <v>108638</v>
+      </c>
+      <c r="W5">
+        <v>2.2000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>44413</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6">
+        <v>799802</v>
+      </c>
+      <c r="E6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" t="s">
+        <v>45</v>
+      </c>
+      <c r="M6">
+        <v>266909</v>
+      </c>
+      <c r="N6">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="O6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="P6" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q6">
+        <v>266973</v>
+      </c>
+      <c r="R6">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="S6">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="T6">
+        <v>46635</v>
+      </c>
+      <c r="U6">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="V6">
+        <v>46546</v>
+      </c>
+      <c r="W6">
+        <v>1.6000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>44416</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7">
+        <v>90974</v>
+      </c>
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L7" t="s">
+        <v>50</v>
+      </c>
+      <c r="M7">
+        <v>44344</v>
+      </c>
+      <c r="N7">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="O7">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="P7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q7">
+        <v>44337</v>
+      </c>
+      <c r="R7">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="S7">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="T7">
+        <v>7853</v>
+      </c>
+      <c r="U7">
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="V7">
+        <v>8025</v>
+      </c>
+      <c r="W7">
+        <v>4.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>44416</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
         <v>28</v>
       </c>
-      <c r="I3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3">
-        <v>15819</v>
-      </c>
-      <c r="N3">
-        <v>0.17960000000000001</v>
-      </c>
-      <c r="O3">
-        <v>1.8499999999999999E-2</v>
-      </c>
-      <c r="P3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q3">
-        <v>15936</v>
-      </c>
-      <c r="R3">
+      <c r="D8">
+        <v>551020</v>
+      </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" t="s">
+        <v>40</v>
+      </c>
+      <c r="J8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" t="s">
+        <v>40</v>
+      </c>
+      <c r="L8" t="s">
+        <v>50</v>
+      </c>
+      <c r="M8">
+        <v>276763</v>
+      </c>
+      <c r="N8">
+        <v>0.17</v>
+      </c>
+      <c r="O8">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="P8" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q8">
+        <v>276537</v>
+      </c>
+      <c r="R8">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="S8">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="T8">
+        <v>46948</v>
+      </c>
+      <c r="U8">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="V8">
+        <v>46681</v>
+      </c>
+      <c r="W8">
+        <v>2.9999999999999997E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>44418</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9">
+        <v>647198</v>
+      </c>
+      <c r="E9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9" t="s">
+        <v>40</v>
+      </c>
+      <c r="K9" t="s">
+        <v>33</v>
+      </c>
+      <c r="L9" t="s">
+        <v>55</v>
+      </c>
+      <c r="M9">
+        <v>323048</v>
+      </c>
+      <c r="N9">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="O9">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="P9" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q9">
+        <v>322944</v>
+      </c>
+      <c r="R9">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="S9">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="T9">
+        <v>53005</v>
+      </c>
+      <c r="U9">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="V9">
+        <v>52894</v>
+      </c>
+      <c r="W9">
+        <v>1.6000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>44419</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10">
+        <v>71618</v>
+      </c>
+      <c r="E10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K10" t="s">
+        <v>33</v>
+      </c>
+      <c r="L10" t="s">
+        <v>60</v>
+      </c>
+      <c r="M10">
+        <v>35840</v>
+      </c>
+      <c r="N10">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="O10">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="P10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q10">
+        <v>35778</v>
+      </c>
+      <c r="R10">
+        <v>0.17</v>
+      </c>
+      <c r="S10">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="T10">
+        <v>6135</v>
+      </c>
+      <c r="U10">
+        <v>3.3E-3</v>
+      </c>
+      <c r="V10">
+        <v>6084</v>
+      </c>
+      <c r="W10">
+        <v>3.5999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>44419</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11">
+        <v>432144</v>
+      </c>
+      <c r="E11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" t="s">
+        <v>59</v>
+      </c>
+      <c r="I11" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K11" t="s">
+        <v>33</v>
+      </c>
+      <c r="L11" t="s">
+        <v>46</v>
+      </c>
+      <c r="M11">
+        <v>216171</v>
+      </c>
+      <c r="N11">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="O11">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="P11" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q11">
+        <v>215973</v>
+      </c>
+      <c r="R11">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="S11">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="T11">
+        <v>35057</v>
+      </c>
+      <c r="U11">
+        <v>2E-3</v>
+      </c>
+      <c r="V11">
+        <v>35151</v>
+      </c>
+      <c r="W11">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>44420</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12">
+        <v>71633</v>
+      </c>
+      <c r="E12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" t="s">
+        <v>63</v>
+      </c>
+      <c r="I12" t="s">
+        <v>40</v>
+      </c>
+      <c r="J12" t="s">
+        <v>32</v>
+      </c>
+      <c r="K12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L12" t="s">
+        <v>64</v>
+      </c>
+      <c r="M12">
+        <v>35810</v>
+      </c>
+      <c r="N12">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="O12">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="P12" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q12">
+        <v>35823</v>
+      </c>
+      <c r="R12">
         <v>0.18099999999999999</v>
       </c>
-      <c r="S3">
-        <v>1.61E-2</v>
-      </c>
-      <c r="T3">
-        <v>15819</v>
-      </c>
-      <c r="U3">
-        <v>6.7999999999999996E-3</v>
-      </c>
-      <c r="V3">
-        <v>15936</v>
-      </c>
-      <c r="W3">
-        <v>5.3E-3</v>
+      <c r="S12">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="T12">
+        <v>6412</v>
+      </c>
+      <c r="U12">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="V12">
+        <v>6375</v>
+      </c>
+      <c r="W12">
+        <v>3.2000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>44420</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13">
+        <v>429412</v>
+      </c>
+      <c r="E13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" t="s">
+        <v>63</v>
+      </c>
+      <c r="I13" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13" t="s">
+        <v>32</v>
+      </c>
+      <c r="K13" t="s">
+        <v>33</v>
+      </c>
+      <c r="L13" t="s">
+        <v>64</v>
+      </c>
+      <c r="M13">
+        <v>214735</v>
+      </c>
+      <c r="N13">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="O13">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="P13" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q13">
+        <v>214677</v>
+      </c>
+      <c r="R13">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="S13">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="T13">
+        <v>36858</v>
+      </c>
+      <c r="U13">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="V13">
+        <v>37123</v>
+      </c>
+      <c r="W13">
+        <v>1E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>